<commit_message>
Updated Writing to Excel
</commit_message>
<xml_diff>
--- a/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
+++ b/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\Homunkulus\Homunkulus\bin\Debug\net6.0-windows\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB48F9BC-6C4F-4C22-A8A8-6C53BFAB89A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4ABD57-8938-4758-B2D0-A488FE15513E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -26,9 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <x:si>
     <x:t xml:space="preserve"> - </x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Tim\Documents\.16151814
+C:\Users\Tim\Documents\.16151814\Vid
+C:\Users\Tim\Documents\.16151814\Vid\Straight</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -362,25 +367,28 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:C1"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="E18" sqref="E18"/>
+      <x:selection activeCell="C19" sqref="C19"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="9.85125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="27.638281" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="10.140625" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="9.85125" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="9.855469" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="92" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1">
         <x:v>44873</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>0</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>1</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added Update to Landingpage and Fixed some little Buggs
</commit_message>
<xml_diff>
--- a/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
+++ b/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\Homunkulus\Homunkulus\bin\Debug\net6.0-windows\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4ABD57-8938-4758-B2D0-A488FE15513E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E210B09E-0463-4F28-A87D-9A8F7BCF8579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="28680" yWindow="5655" windowWidth="29040" windowHeight="16440" firstSheet="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Backupplans" sheetId="1" r:id="rId1"/>
+    <x:sheet name="General" sheetId="2" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
     <x:t xml:space="preserve"> - </x:t>
   </x:si>
@@ -35,6 +36,25 @@
 C:\Users\Tim\Documents\.16151814\Vid
 C:\Users\Tim\Documents\.16151814\Vid\Straight</x:t>
   </x:si>
+  <x:si>
+    <x:t>G:\</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Tim\Documents\.16151814
+C:\Users\Tim\Documents\.Autos
+C:\Users\Tim\Documents\.Bewerbungsunterlagen
+C:\Users\Tim\Documents\.Buchhaltung
+C:\Users\Tim\Documents\.Dounjinshi
+C:\Users\Tim\Documents\.Minecraft_Server
+C:\Users\Tim\Documents\.Projekte
+C:\Users\Tim\Documents\GitHub
+C:\Users\Tim\Pictures
+C:\Users\Tim\Videos
+C:\Users\Tim\Music</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Times Executed </x:t>
+  </x:si>
 </x:sst>
 </file>
 
@@ -43,8 +63,16 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="2" x14ac:knownFonts="1">
+  <x:fonts count="3" x14ac:knownFonts="1">
     <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
       <x:sz val="11"/>
       <x:color theme="1"/>
       <x:name val="Calibri"/>
@@ -76,15 +104,33 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="7">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment horizontal="center" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment vertical="center" wrapText="1"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <x:alignment horizontal="center"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -369,27 +415,43 @@
   </x:sheetPr>
   <x:dimension ref="A1:C1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="C19" sqref="C19"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="C15" sqref="C15"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="27.638281" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="28.280938" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="10.140625" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="2" width="9.855469" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="92" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="9.855469" style="2" customWidth="1"/>
+    <x:col min="3" max="3" width="117.140625" style="3" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1">
         <x:v>44873</x:v>
       </x:c>
-      <x:c r="B1" s="0" t="s">
+      <x:c r="B1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
+      <x:c r="C1" s="3" t="s">
         <x:v>1</x:v>
       </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="1">
+        <x:v>44875</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:3">
+      <x:c r="A15" s="4" t="s"/>
+      <x:c r="B15" s="2" t="s"/>
+      <x:c r="C15" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -398,4 +460,38 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{1166E000-C9FA-4053-A65F-80DE0A59A45E}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A2:B2"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="L21" sqref="L21"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="15.285156" style="5" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="11.425781" style="6" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="5" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B2" s="6" t="n">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.787401575" bottom="0.787401575" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Change the save from .CSV to .XML
</commit_message>
<xml_diff>
--- a/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
+++ b/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <x:si>
     <x:t xml:space="preserve"> - </x:t>
   </x:si>
@@ -51,6 +51,12 @@
 C:\Users\Tim\Pictures
 C:\Users\Tim\Videos
 C:\Users\Tim\Music</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Deine Mudad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>asdddsasssddar</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Times Executed </x:t>
@@ -419,7 +425,7 @@
       <x:selection activeCell="C15" sqref="C15"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="28.280938" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="28.991563" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="9.855469" style="2" customWidth="1"/>
@@ -446,6 +452,17 @@
       </x:c>
       <x:c r="C2" s="3" t="s">
         <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="1">
+        <x:v>44894</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="3" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
@@ -481,7 +498,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A2" s="5" t="s">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="6" t="n">
         <x:v>1</x:v>

</xml_diff>

<commit_message>
Added Write to Xml
</commit_message>
<xml_diff>
--- a/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
+++ b/Homunkulus/bin/Debug/net6.0-windows/Resources/database.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <x:si>
     <x:t xml:space="preserve"> - </x:t>
   </x:si>
@@ -57,6 +57,17 @@
   </x:si>
   <x:si>
     <x:t>asdddsasssddar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>G:\Backup\</x:t>
+  </x:si>
+  <x:si>
+    <x:t>C:\Users\Tim\Documents\16151814
+C:\Users\Tim\Documents\Autos
+C:\Users\Tim\Documents\Bewerbungsuntlagen
+C:\Users\Tim\Documents\Buchaltung
+C:\Users\Tim\Documents\Dounjinshi
+C:\Users\Tim\Documents\GitHub</x:t>
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Times Executed </x:t>
@@ -425,7 +436,7 @@
       <x:selection activeCell="C15" sqref="C15"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="28.991563" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="29.702188" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="9.855469" style="2" customWidth="1"/>
@@ -463,6 +474,17 @@
       </x:c>
       <x:c r="C3" s="3" t="s">
         <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="1">
+        <x:v>44896</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:3">
@@ -498,7 +520,7 @@
   <x:sheetData>
     <x:row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A2" s="5" t="s">
-        <x:v>6</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B2" s="6" t="n">
         <x:v>1</x:v>

</xml_diff>